<commit_message>
Fix wires, svg to png, add vertical wiring
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -4,16 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tâches" sheetId="1" r:id="rId1"/>
-    <sheet name="Totaux" sheetId="3" r:id="rId2"/>
-    <sheet name="Sources" sheetId="2" r:id="rId3"/>
+    <sheet name="Feuil1" sheetId="4" r:id="rId1"/>
+    <sheet name="Tâches" sheetId="1" r:id="rId2"/>
+    <sheet name="Totaux" sheetId="3" r:id="rId3"/>
+    <sheet name="Sources" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t>Index</t>
   </si>
@@ -164,6 +166,84 @@
   </si>
   <si>
     <t>Planification détaillée en sprints et tâches</t>
+  </si>
+  <si>
+    <t>Discussion avec le chef de projet</t>
+  </si>
+  <si>
+    <t>Mise en forme</t>
+  </si>
+  <si>
+    <t>Complétion du glossaire, de l'analyse et de la conception</t>
+  </si>
+  <si>
+    <t>Refonte des maquettes, flowcharts</t>
+  </si>
+  <si>
+    <t>Lancement du projet Unity</t>
+  </si>
+  <si>
+    <t>https://bgolus.medium.com/progressing-in-circles-13452434fdb9, https://docs.unity3d.com/ScriptReference/LineRenderer-colorGradient.html</t>
+  </si>
+  <si>
+    <t>https://docs.unity3d.com/Manual/class-LineRenderer.html</t>
+  </si>
+  <si>
+    <t>Développement de l'interface</t>
+  </si>
+  <si>
+    <t>Développement des portes</t>
+  </si>
+  <si>
+    <t>Développement des câbles</t>
+  </si>
+  <si>
+    <t>Reconsidération de la logique programmatoire inhérente au projet</t>
+  </si>
+  <si>
+    <t>Fixing du code. Recréation de la logique IO</t>
+  </si>
+  <si>
+    <t>Logique des câbles</t>
+  </si>
+  <si>
+    <t>Refactoring du code</t>
+  </si>
+  <si>
+    <t>Visite de Mr. Gehrig</t>
+  </si>
+  <si>
+    <t>Je me rends compte que tout le code que j'ai fait est trop compliqué. Je vais tout reconceptualiser.</t>
+  </si>
+  <si>
+    <t>Somme de Index</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Fin de refacotring du code.</t>
+  </si>
+  <si>
+    <t>C'est bon ça marche :)</t>
+  </si>
+  <si>
+    <t>Photoshoppage de tous les composants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour pouvoir ensuite modifier leur couleur dynamiquement </t>
+  </si>
+  <si>
+    <t>Adaptation des SVG pour Unity</t>
   </si>
 </sst>
 </file>
@@ -247,7 +327,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Auteur" refreshedDate="44319.703383217595" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Auteur" refreshedDate="44333.702921296295" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I39" sheet="Tâches"/>
   </cacheSource>
@@ -294,34 +374,220 @@
         <n v="38"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2021-05-03T00:00:00" maxDate="2021-05-04T00:00:00"/>
+    <cacheField name="Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2021-05-03T00:00:00" maxDate="2021-05-18T00:00:00"/>
     </cacheField>
-    <cacheField name="Début" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T08:08:00" maxDate="1899-12-30T16:04:00"/>
+    <cacheField name="Début" numFmtId="20">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T08:03:00" maxDate="1899-12-30T16:04:00"/>
     </cacheField>
-    <cacheField name="Fin" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T08:13:00" maxDate="1899-12-30T16:52:00"/>
+    <cacheField name="Fin" numFmtId="20">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T08:13:00" maxDate="1899-12-30T16:55:00"/>
     </cacheField>
     <cacheField name="Durée" numFmtId="20">
-      <sharedItems containsDate="1" containsMixedTypes="1" minDate="1899-12-30T00:03:00" maxDate="1899-12-30T01:36:00"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:03:00" maxDate="1899-12-30T03:22:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
-      <sharedItems containsBlank="1" count="4">
+      <sharedItems containsBlank="1" count="6">
         <s v="Analyse"/>
         <s v="Misc."/>
         <s v="Documentation"/>
-        <m/>
+        <s v="Conception"/>
+        <s v="Réalisation"/>
+        <m u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Tâche" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Commentaire" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sources" numFmtId="0">
       <sharedItems containsBlank="1" longText="1"/>
     </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Auteur" refreshedDate="44333.70420925926" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="41">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:I42" sheet="Tâches"/>
+  </cacheSource>
+  <cacheFields count="10">
+    <cacheField name="Index" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="41"/>
+    </cacheField>
+    <cacheField name="Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2021-05-03T00:00:00" maxDate="2021-05-18T00:00:00"/>
+    </cacheField>
+    <cacheField name="Début" numFmtId="20">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T08:03:00" maxDate="1899-12-30T16:04:00"/>
+    </cacheField>
+    <cacheField name="Fin" numFmtId="20">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T08:13:00" maxDate="1899-12-30T16:55:00"/>
+    </cacheField>
+    <cacheField name="Durée" numFmtId="20">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:03:00" maxDate="1899-12-30T03:22:00" count="35">
+        <d v="1899-12-30T00:05:00"/>
+        <d v="1899-12-30T00:11:00"/>
+        <d v="1899-12-30T00:28:00"/>
+        <d v="1899-12-30T00:35:00"/>
+        <d v="1899-12-30T00:23:00"/>
+        <d v="1899-12-30T00:22:00"/>
+        <d v="1899-12-30T00:03:00"/>
+        <d v="1899-12-30T00:31:00"/>
+        <d v="1899-12-30T00:13:00"/>
+        <d v="1899-12-30T00:44:00"/>
+        <d v="1899-12-30T01:36:00"/>
+        <d v="1899-12-30T00:07:00"/>
+        <d v="1899-12-30T00:30:00"/>
+        <d v="1899-12-30T00:48:00"/>
+        <d v="1899-12-30T00:27:00"/>
+        <d v="1899-12-30T02:15:00"/>
+        <d v="1899-12-30T00:38:00"/>
+        <d v="1899-12-30T00:33:00"/>
+        <d v="1899-12-30T00:16:00"/>
+        <d v="1899-12-30T01:12:00"/>
+        <d v="1899-12-30T00:19:00"/>
+        <d v="1899-12-30T02:19:00"/>
+        <d v="1899-12-30T03:18:00"/>
+        <d v="1899-12-30T03:22:00"/>
+        <d v="1899-12-30T01:17:00"/>
+        <d v="1899-12-30T02:24:00"/>
+        <d v="1899-12-30T01:35:00"/>
+        <d v="1899-12-30T01:32:00"/>
+        <d v="1899-12-30T02:20:00"/>
+        <d v="1899-12-30T00:45:00"/>
+        <d v="1899-12-30T00:37:00"/>
+        <d v="1899-12-30T00:43:00"/>
+        <d v="1899-12-30T01:45:00"/>
+        <d v="1899-12-30T01:13:00"/>
+        <d v="1899-12-30T01:30:00"/>
+      </sharedItems>
+      <fieldGroup par="9" base="4">
+        <rangePr groupBy="minutes" startDate="1899-12-30T00:03:00" endDate="1899-12-30T03:22:00"/>
+        <groupItems count="62">
+          <s v="&lt;00.01.1900"/>
+          <s v=":00"/>
+          <s v=":01"/>
+          <s v=":02"/>
+          <s v=":03"/>
+          <s v=":04"/>
+          <s v=":05"/>
+          <s v=":06"/>
+          <s v=":07"/>
+          <s v=":08"/>
+          <s v=":09"/>
+          <s v=":10"/>
+          <s v=":11"/>
+          <s v=":12"/>
+          <s v=":13"/>
+          <s v=":14"/>
+          <s v=":15"/>
+          <s v=":16"/>
+          <s v=":17"/>
+          <s v=":18"/>
+          <s v=":19"/>
+          <s v=":20"/>
+          <s v=":21"/>
+          <s v=":22"/>
+          <s v=":23"/>
+          <s v=":24"/>
+          <s v=":25"/>
+          <s v=":26"/>
+          <s v=":27"/>
+          <s v=":28"/>
+          <s v=":29"/>
+          <s v=":30"/>
+          <s v=":31"/>
+          <s v=":32"/>
+          <s v=":33"/>
+          <s v=":34"/>
+          <s v=":35"/>
+          <s v=":36"/>
+          <s v=":37"/>
+          <s v=":38"/>
+          <s v=":39"/>
+          <s v=":40"/>
+          <s v=":41"/>
+          <s v=":42"/>
+          <s v=":43"/>
+          <s v=":44"/>
+          <s v=":45"/>
+          <s v=":46"/>
+          <s v=":47"/>
+          <s v=":48"/>
+          <s v=":49"/>
+          <s v=":50"/>
+          <s v=":51"/>
+          <s v=":52"/>
+          <s v=":53"/>
+          <s v=":54"/>
+          <s v=":55"/>
+          <s v=":56"/>
+          <s v=":57"/>
+          <s v=":58"/>
+          <s v=":59"/>
+          <s v="&gt;00.01.1900"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+    <cacheField name="Type" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Analyse"/>
+        <s v="Misc."/>
+        <s v="Documentation"/>
+        <s v="Conception"/>
+        <s v="Réalisation"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Tâche" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Commentaire" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
     <cacheField name="Sources" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1" longText="1"/>
+    </cacheField>
+    <cacheField name="Heures" numFmtId="0" databaseField="0">
+      <fieldGroup base="4">
+        <rangePr groupBy="hours" startDate="1899-12-30T00:03:00" endDate="1899-12-30T03:22:00"/>
+        <groupItems count="26">
+          <s v="&lt;00.01.1900"/>
+          <s v="00"/>
+          <s v="01"/>
+          <s v="02"/>
+          <s v="03"/>
+          <s v="04"/>
+          <s v="05"/>
+          <s v="06"/>
+          <s v="07"/>
+          <s v="08"/>
+          <s v="09"/>
+          <s v="10"/>
+          <s v="11"/>
+          <s v="12"/>
+          <s v="13"/>
+          <s v="14"/>
+          <s v="15"/>
+          <s v="16"/>
+          <s v="17"/>
+          <s v="18"/>
+          <s v="19"/>
+          <s v="20"/>
+          <s v="21"/>
+          <s v="22"/>
+          <s v="23"/>
+          <s v="&gt;00.01.1900"/>
+        </groupItems>
+      </fieldGroup>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -430,8 +696,8 @@
     <d v="1899-12-30T00:13:00"/>
     <x v="0"/>
     <s v="Recherche d'informations sur le sujet"/>
+    <m/>
     <s v=" 1. https://www.allaboutcircuits.com/textbook/digital/chpt-7/converting-truth-tables-boolean-expressions/#:~:text=Sum%2DOf%2DProducts%2C%20or%20SOP%2C%20Boolean%20expressions%20may,truth%20table%20as%20a%20whole._x000a_2. https://www.electronics-tutorials.ws/boolean/product-of-sum.html_x000a_3. https://www.electricaltechnology.org/2018/05/sum-of-product-sop-product-of-sum-pos.html_x000a_4. https://fr.wikipedia.org/wiki/Alg%C3%A8bre_de_Boole_(logique)_x000a_5. http://lycees.ac-rouen.fr/modeste-leroy/spip/IMG/pdf/_algebre_de_boole.pdf_x000a_6. https://sourceforge.net/projects/gkmap/_x000a_7. http://k-map.sourceforge.net/_x000a_8. https://www.dcode.fr/boolean-expressions-calculator_x000a_9. https://www.youtube.com/watch?v=QZwneRb-zqA"/>
-    <m/>
   </r>
   <r>
     <x v="9"/>
@@ -485,270 +751,726 @@
     <d v="1899-12-30T00:48:00"/>
     <x v="2"/>
     <s v="Planifaication initiale et Début du dossier de conception"/>
+    <m/>
     <s v="https://vertabelo.com/blog/crow-s-foot-notation/"/>
-    <m/>
   </r>
   <r>
     <x v="14"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T08:05:00"/>
+    <d v="1899-12-30T08:32:00"/>
+    <d v="1899-12-30T00:27:00"/>
+    <x v="2"/>
+    <s v="Convention de nommage, versioning"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="15"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T09:07:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <d v="1899-12-30T00:28:00"/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
+    <s v="Maquettes"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="16"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <d v="1899-12-30T02:15:00"/>
+    <x v="3"/>
+    <s v="Maquettes"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="17"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T14:08:00"/>
+    <d v="1899-12-30T00:38:00"/>
+    <x v="3"/>
+    <s v="Palette de couleur"/>
+    <s v="Aide de Mr. Wyssa sur le MCD"/>
+    <m/>
+  </r>
+  <r>
+    <x v="18"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T14:10:00"/>
+    <d v="1899-12-30T14:43:00"/>
+    <d v="1899-12-30T00:33:00"/>
+    <x v="2"/>
+    <s v="Documentation des maquettes"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="19"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T14:44:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <d v="1899-12-30T00:16:00"/>
+    <x v="2"/>
+    <s v="Planification détaillée en sprints et tâches"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="20"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T15:30:00"/>
+    <d v="1899-12-30T16:05:00"/>
+    <d v="1899-12-30T00:35:00"/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="21"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T08:05:00"/>
+    <d v="1899-12-30T09:17:00"/>
+    <d v="1899-12-30T01:12:00"/>
+    <x v="1"/>
+    <s v="Discussion avec le chef de projet"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="22"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T09:17:00"/>
+    <d v="1899-12-30T09:36:00"/>
+    <d v="1899-12-30T00:19:00"/>
+    <x v="2"/>
+    <s v="Mise en forme"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="23"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T09:56:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <d v="1899-12-30T02:19:00"/>
+    <x v="2"/>
+    <s v="Complétion du glossaire, de l'analyse et de la conception"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="24"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T13:32:00"/>
+    <d v="1899-12-30T16:50:00"/>
+    <d v="1899-12-30T03:18:00"/>
+    <x v="3"/>
+    <s v="Refonte des maquettes, flowcharts"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="25"/>
+    <d v="2021-05-07T00:00:00"/>
+    <d v="1899-12-30T08:03:00"/>
+    <d v="1899-12-30T11:25:00"/>
+    <d v="1899-12-30T03:22:00"/>
+    <x v="4"/>
+    <s v="Lancement du projet Unity"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="26"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T08:18:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <d v="1899-12-30T01:17:00"/>
+    <x v="4"/>
+    <s v="Développement de l'interface"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="27"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T09:51:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <d v="1899-12-30T02:24:00"/>
+    <x v="4"/>
+    <s v="Développement de l'interface"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="28"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:05:00"/>
+    <d v="1899-12-30T01:35:00"/>
+    <x v="4"/>
+    <s v="Développement des portes"/>
+    <s v="https://bgolus.medium.com/progressing-in-circles-13452434fdb9, https://docs.unity3d.com/ScriptReference/LineRenderer-colorGradient.html"/>
+    <m/>
+  </r>
+  <r>
+    <x v="29"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T15:20:00"/>
+    <d v="1899-12-30T16:55:00"/>
+    <d v="1899-12-30T01:35:00"/>
+    <x v="4"/>
+    <s v="Développement des portes"/>
+    <s v="https://docs.unity3d.com/Manual/class-LineRenderer.html"/>
+    <m/>
+  </r>
+  <r>
+    <x v="30"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T08:03:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <d v="1899-12-30T01:32:00"/>
+    <x v="4"/>
+    <s v="Développement des portes"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="31"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T09:52:00"/>
+    <d v="1899-12-30T12:12:00"/>
+    <d v="1899-12-30T02:20:00"/>
+    <x v="4"/>
+    <s v="Développement des câbles"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="32"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:06:00"/>
+    <d v="1899-12-30T01:36:00"/>
+    <x v="4"/>
+    <s v="Développement des câbles"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="33"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T15:20:00"/>
+    <d v="1899-12-30T16:05:00"/>
+    <d v="1899-12-30T00:45:00"/>
+    <x v="4"/>
+    <s v="Développement des câbles"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="34"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T08:15:00"/>
+    <d v="1899-12-30T08:52:00"/>
+    <d v="1899-12-30T00:37:00"/>
+    <x v="3"/>
+    <s v="Reconsidération de la logique programmatoire inhérente au projet"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="35"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T08:52:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <d v="1899-12-30T00:43:00"/>
+    <x v="4"/>
+    <s v="Fixing du code. Recréation de la logique IO"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="36"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T09:52:00"/>
+    <d v="1899-12-30T10:29:00"/>
+    <d v="1899-12-30T00:37:00"/>
+    <x v="4"/>
+    <s v="Logique des câbles"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="37"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T10:30:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <d v="1899-12-30T01:45:00"/>
+    <x v="4"/>
+    <s v="Logique des câbles"/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="41">
+  <r>
+    <n v="1"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T08:08:00"/>
+    <d v="1899-12-30T08:13:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Découverte du CDC"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="2"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T08:14:00"/>
+    <d v="1899-12-30T08:25:00"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Mise en place du GIT, début d'analyse"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="3"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T08:30:00"/>
+    <d v="1899-12-30T08:58:00"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Discussion sur le CDC avec Mr. Melly et Mr. Gehrig"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="4"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T09:00:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="Création de la planification initiale"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="5"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T09:55:00"/>
+    <d v="1899-12-30T10:18:00"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Création de la planification initiale"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="6"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T10:19:00"/>
+    <d v="1899-12-30T10:41:00"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Création du projet Unity et implémentation du GIT"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="7"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T10:42:00"/>
+    <d v="1899-12-30T10:45:00"/>
+    <x v="6"/>
+    <x v="2"/>
+    <s v="Création du fichier Word pour le rapport "/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="8"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T10:46:00"/>
+    <d v="1899-12-30T11:17:00"/>
+    <x v="7"/>
+    <x v="0"/>
+    <s v="Mise en place du Kanban sur GitHub et des sprints"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="9"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T11:18:00"/>
+    <d v="1899-12-30T11:31:00"/>
+    <x v="8"/>
+    <x v="0"/>
+    <s v="Recherche d'informations sur le sujet"/>
+    <m/>
+    <s v=" 1. https://www.allaboutcircuits.com/textbook/digital/chpt-7/converting-truth-tables-boolean-expressions/#:~:text=Sum%2DOf%2DProducts%2C%20or%20SOP%2C%20Boolean%20expressions%20may,truth%20table%20as%20a%20whole._x000a_2. https://www.electronics-tutorials.ws/boolean/product-of-sum.html_x000a_3. https://www.electricaltechnology.org/2018/05/sum-of-product-sop-product-of-sum-pos.html_x000a_4. https://fr.wikipedia.org/wiki/Alg%C3%A8bre_de_Boole_(logique)_x000a_5. http://lycees.ac-rouen.fr/modeste-leroy/spip/IMG/pdf/_algebre_de_boole.pdf_x000a_6. https://sourceforge.net/projects/gkmap/_x000a_7. http://k-map.sourceforge.net/_x000a_8. https://www.dcode.fr/boolean-expressions-calculator_x000a_9. https://www.youtube.com/watch?v=QZwneRb-zqA"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T11:32:00"/>
+    <d v="1899-12-30T12:16:00"/>
+    <x v="9"/>
+    <x v="2"/>
+    <s v="Documentation du projet"/>
+    <s v="Introduction au TPI, buts, objectifs"/>
+    <m/>
+  </r>
+  <r>
+    <n v="11"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:06:00"/>
+    <x v="10"/>
+    <x v="2"/>
+    <s v="Difficultés attendues et Glossaire"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T15:25:00"/>
+    <d v="1899-12-30T15:32:00"/>
+    <x v="11"/>
+    <x v="2"/>
+    <s v="Finition du glossaire"/>
+    <s v="Pour l'instant il y a 45 entrées."/>
+    <m/>
+  </r>
+  <r>
+    <n v="13"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T15:33:00"/>
+    <d v="1899-12-30T16:03:00"/>
+    <x v="12"/>
+    <x v="2"/>
+    <s v="Mise en forme du rapport et table des matières"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="14"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T16:04:00"/>
+    <d v="1899-12-30T16:52:00"/>
+    <x v="13"/>
+    <x v="2"/>
+    <s v="Planifaication initiale et Début du dossier de conception"/>
+    <m/>
+    <s v="https://vertabelo.com/blog/crow-s-foot-notation/"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T08:05:00"/>
+    <d v="1899-12-30T08:32:00"/>
+    <x v="14"/>
+    <x v="2"/>
+    <s v="Convention de nommage, versioning"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="16"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T09:07:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="Maquettes"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="17"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T12:15:00"/>
     <x v="15"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
+    <s v="Maquettes"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="18"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T14:08:00"/>
     <x v="16"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
+    <s v="Palette de couleur"/>
+    <s v="Aide de Mr. Wyssa sur le MCD"/>
+    <m/>
+  </r>
+  <r>
+    <n v="19"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T14:10:00"/>
+    <d v="1899-12-30T14:43:00"/>
     <x v="17"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
+    <x v="2"/>
+    <s v="Documentation des maquettes"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="20"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T14:44:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <x v="18"/>
+    <x v="2"/>
+    <s v="Planification détaillée en sprints et tâches"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="21"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T15:30:00"/>
+    <d v="1899-12-30T16:05:00"/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="18"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="22"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T08:05:00"/>
+    <d v="1899-12-30T09:17:00"/>
+    <x v="19"/>
+    <x v="1"/>
+    <s v="Discussion avec le chef de projet"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="23"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T09:17:00"/>
+    <d v="1899-12-30T09:36:00"/>
+    <x v="20"/>
+    <x v="2"/>
+    <s v="Mise en forme"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="24"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T09:56:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <x v="21"/>
+    <x v="2"/>
+    <s v="Complétion du glossaire, de l'analyse et de la conception"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="25"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T13:32:00"/>
+    <d v="1899-12-30T16:50:00"/>
+    <x v="22"/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="19"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
+    <s v="Refonte des maquettes, flowcharts"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="26"/>
+    <d v="2021-05-07T00:00:00"/>
+    <d v="1899-12-30T08:03:00"/>
+    <d v="1899-12-30T11:25:00"/>
+    <x v="23"/>
+    <x v="4"/>
+    <s v="Lancement du projet Unity"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="27"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T08:18:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="24"/>
+    <x v="4"/>
+    <s v="Développement de l'interface"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="28"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T09:51:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <x v="25"/>
+    <x v="4"/>
+    <s v="Développement de l'interface"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="29"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:05:00"/>
+    <x v="26"/>
+    <x v="4"/>
+    <s v="Développement des portes"/>
+    <s v="https://bgolus.medium.com/progressing-in-circles-13452434fdb9, https://docs.unity3d.com/ScriptReference/LineRenderer-colorGradient.html"/>
+    <m/>
+  </r>
+  <r>
+    <n v="30"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T15:20:00"/>
+    <d v="1899-12-30T16:55:00"/>
+    <x v="26"/>
+    <x v="4"/>
+    <s v="Développement des portes"/>
+    <s v="https://docs.unity3d.com/Manual/class-LineRenderer.html"/>
+    <m/>
+  </r>
+  <r>
+    <n v="31"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T08:03:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="27"/>
+    <x v="4"/>
+    <s v="Développement des portes"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="32"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T09:52:00"/>
+    <d v="1899-12-30T12:12:00"/>
+    <x v="28"/>
+    <x v="4"/>
+    <s v="Développement des câbles"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="33"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:06:00"/>
+    <x v="10"/>
+    <x v="4"/>
+    <s v="Développement des câbles"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="34"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T15:20:00"/>
+    <d v="1899-12-30T16:05:00"/>
+    <x v="29"/>
+    <x v="4"/>
+    <s v="Développement des câbles"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="35"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T08:15:00"/>
+    <d v="1899-12-30T08:52:00"/>
+    <x v="30"/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="20"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="21"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="22"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="23"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="24"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="25"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="26"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="27"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="28"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="29"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
+    <s v="Reconsidération de la logique programmatoire inhérente au projet"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="36"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T08:52:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="31"/>
+    <x v="4"/>
+    <s v="Fixing du code. Recréation de la logique IO"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="37"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T09:52:00"/>
+    <d v="1899-12-30T10:29:00"/>
     <x v="30"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="31"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
+    <x v="4"/>
+    <s v="Logique des câbles"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="38"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T10:30:00"/>
+    <d v="1899-12-30T12:15:00"/>
     <x v="32"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
+    <x v="4"/>
+    <s v="Logique des câbles"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="39"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T13:32:00"/>
+    <d v="1899-12-30T14:45:00"/>
     <x v="33"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
+    <x v="4"/>
+    <s v="Refactoring du code"/>
+    <s v="Je me rends compte que tout le code que j'ai fait est trop compliqué. Je vais tout reconceptualiser."/>
+    <m/>
+  </r>
+  <r>
+    <n v="40"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T14:45:00"/>
+    <d v="1899-12-30T15:15:00"/>
+    <x v="12"/>
+    <x v="1"/>
+    <s v="Visite de Mr. Gehrig"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="41"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T15:20:00"/>
+    <d v="1899-12-30T16:50:00"/>
     <x v="34"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="35"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="36"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="37"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=""/>
-    <x v="3"/>
-    <m/>
+    <x v="4"/>
+    <s v="Refactoring du code"/>
     <m/>
     <m/>
   </r>
@@ -756,8 +1478,183 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField numFmtId="20" showAll="0"/>
+    <pivotField numFmtId="20" showAll="0"/>
+    <pivotField axis="axisCol" numFmtId="20" showAll="0">
+      <items count="63">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="26">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="25"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="9"/>
+    <field x="4"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Somme de Index" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:E19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A3:E26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
       <items count="39">
@@ -807,11 +1704,13 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="5">
+      <items count="7">
         <item x="0"/>
         <item x="1"/>
+        <item h="1" m="1" x="5"/>
+        <item x="2"/>
         <item h="1" x="3"/>
-        <item x="2"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -822,7 +1721,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="15">
+  <rowItems count="22">
     <i>
       <x/>
     </i>
@@ -864,6 +1763,27 @@
     </i>
     <i>
       <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
     </i>
     <i t="grand">
       <x/>
@@ -1166,10 +2086,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A3:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="22" width="3.5703125" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" customWidth="1"/>
+    <col min="24" max="30" width="3.5703125" customWidth="1"/>
+    <col min="31" max="31" width="4.85546875" customWidth="1"/>
+    <col min="32" max="34" width="3.5703125" customWidth="1"/>
+    <col min="35" max="35" width="4.85546875" customWidth="1"/>
+    <col min="36" max="36" width="3.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5">
+        <v>69</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5">
+        <v>25</v>
+      </c>
+      <c r="F7" s="5">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5">
+        <v>160</v>
+      </c>
+      <c r="C8" s="5">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5">
+        <v>24</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5">
+        <v>22</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>107</v>
+      </c>
+      <c r="C10" s="5">
+        <v>268</v>
+      </c>
+      <c r="D10" s="5">
+        <v>60</v>
+      </c>
+      <c r="E10" s="5">
+        <v>26</v>
+      </c>
+      <c r="F10" s="5">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5">
+        <v>408</v>
+      </c>
+      <c r="C11" s="5">
+        <v>301</v>
+      </c>
+      <c r="D11" s="5">
+        <v>101</v>
+      </c>
+      <c r="E11" s="5">
+        <v>51</v>
+      </c>
+      <c r="F11" s="5">
+        <v>861</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +2262,7 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="7" max="7" width="60" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="87.5703125" customWidth="1"/>
     <col min="9" max="9" width="84.28515625" customWidth="1"/>
   </cols>
@@ -1238,7 +2323,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A39" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A49" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -1251,7 +2336,7 @@
         <v>0.35069444444444442</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E39" si="1">IF(OR(ISBLANK(D3),ISBLANK(C3)),"",D3-C3)</f>
+        <f t="shared" ref="E3:E45" si="1">IF(OR(ISBLANK(D3),ISBLANK(C3)),"",D3-C3)</f>
         <v>7.6388888888889173E-3</v>
       </c>
       <c r="F3" t="s">
@@ -1598,7 +2683,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1623,7 +2708,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1648,7 +2733,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1676,7 +2761,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1701,7 +2786,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1726,7 +2811,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1744,175 +2829,619 @@
         <f t="shared" si="1"/>
         <v>2.4305555555555469E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="E23" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>44322</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="1"/>
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="E24" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>44322</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3194444444444398E-2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="E25" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>44322</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.41388888888888892</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="1"/>
+        <v>9.6527777777777712E-2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="E26" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>44322</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13749999999999996</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="E27" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>44323</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14027777777777772</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="E28" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>44326</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.34583333333333338</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="1"/>
+        <v>5.3472222222222199E-2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E29" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>44326</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.41041666666666665</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E30" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>44326</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="1"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E31" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>44326</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="1"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="E32" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>44327</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="1"/>
+        <v>6.3888888888888884E-2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="E33" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>44327</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.41111111111111115</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="1"/>
+        <v>9.7222222222222154E-2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>53</v>
+      </c>
+      <c r="I33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="E34" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>44327</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="1"/>
+        <v>6.6666666666666652E-2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="E35" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>44327</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1249999999999889E-2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="E36" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>44333</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.34375</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.36944444444444446</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="1"/>
+        <v>2.5694444444444464E-2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="E37" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>44333</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.36944444444444446</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="1"/>
+        <v>2.9861111111111116E-2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="E38" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>44333</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.41111111111111115</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.4368055555555555</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="1"/>
+        <v>2.5694444444444353E-2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="E39" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B39" s="1">
+        <v>44333</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="1"/>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
+        <v>44333</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="1"/>
+        <v>5.0694444444444486E-2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" t="s">
+        <v>57</v>
+      </c>
+      <c r="H40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44333</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44333</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="1"/>
+        <v>6.2499999999999889E-2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44334</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="1"/>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" t="s">
+        <v>65</v>
+      </c>
+      <c r="H43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44334</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6805555555555591E-2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" t="s">
+        <v>67</v>
+      </c>
+      <c r="H44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.41180555555555554</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="1"/>
+        <v>9.8611111111111094E-2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +3456,7 @@
           <x14:formula1>
             <xm:f>Sources!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F39</xm:sqref>
+          <xm:sqref>F2:F58</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1935,12 +3464,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E19"/>
+  <dimension ref="A3:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,20 +3689,111 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="4">
+        <v>15</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1.8749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="E20" s="5">
+        <v>2.2916666666666669E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1.1111111111111112E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="E22" s="5">
+        <v>2.4305555555555556E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5">
+        <v>4.9999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="E24" s="5">
+        <v>1.3194444444444444E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5">
+        <v>9.6527777777777768E-2</v>
+      </c>
+      <c r="E25" s="5">
+        <v>9.6527777777777768E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="6">
         <v>8.1944444444444445E-2</v>
       </c>
-      <c r="C19" s="6">
-        <v>1.9444444444444445E-2</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0.1736111111111111</v>
-      </c>
-      <c r="E19" s="6">
-        <v>0.27500000000000002</v>
+      <c r="C26" s="6">
+        <v>6.9444444444444448E-2</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.36041666666666666</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.51180555555555562</v>
       </c>
     </row>
   </sheetData>
@@ -2182,7 +3802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>

</xml_diff>

<commit_message>
Wire clarification + input outputs canvas
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -14,8 +14,8 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId5"/>
-    <pivotCache cacheId="15" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="5" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="72">
   <si>
     <t>Index</t>
   </si>
@@ -242,6 +242,15 @@
   <si>
     <t>Rédaction d'un certain nombre de problèmes rencontrés</t>
   </si>
+  <si>
+    <t>Suppression des câbles et amélioration de la visibilité</t>
+  </si>
+  <si>
+    <t>Inputs et outputs du canevas</t>
+  </si>
+  <si>
+    <t>synérgie canevas et inputs</t>
+  </si>
 </sst>
 </file>
 
@@ -249,7 +258,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -302,112 +311,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
@@ -426,94 +354,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Auteur" refreshedDate="44336.511992939813" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:I39" sheet="Tâches"/>
-  </cacheSource>
-  <cacheFields count="9">
-    <cacheField name="Index" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="38" count="38">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="3"/>
-        <n v="4"/>
-        <n v="5"/>
-        <n v="6"/>
-        <n v="7"/>
-        <n v="8"/>
-        <n v="9"/>
-        <n v="10"/>
-        <n v="11"/>
-        <n v="12"/>
-        <n v="13"/>
-        <n v="14"/>
-        <n v="15"/>
-        <n v="16"/>
-        <n v="17"/>
-        <n v="18"/>
-        <n v="19"/>
-        <n v="20"/>
-        <n v="21"/>
-        <n v="22"/>
-        <n v="23"/>
-        <n v="24"/>
-        <n v="25"/>
-        <n v="26"/>
-        <n v="27"/>
-        <n v="28"/>
-        <n v="29"/>
-        <n v="30"/>
-        <n v="31"/>
-        <n v="32"/>
-        <n v="33"/>
-        <n v="34"/>
-        <n v="35"/>
-        <n v="36"/>
-        <n v="37"/>
-        <n v="38"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2021-05-03T00:00:00" maxDate="2021-05-18T00:00:00"/>
-    </cacheField>
-    <cacheField name="Début" numFmtId="20">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T08:03:00" maxDate="1899-12-30T16:04:00"/>
-    </cacheField>
-    <cacheField name="Fin" numFmtId="20">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T08:13:00" maxDate="1899-12-30T16:55:00"/>
-    </cacheField>
-    <cacheField name="Durée" numFmtId="20">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:03:00" maxDate="1899-12-30T03:22:00"/>
-    </cacheField>
-    <cacheField name="Type" numFmtId="0">
-      <sharedItems containsBlank="1" count="6">
-        <s v="Analyse"/>
-        <s v="Misc."/>
-        <s v="Documentation"/>
-        <s v="Conception"/>
-        <s v="Réalisation"/>
-        <m u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Tâche" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Commentaire" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Sources" numFmtId="0">
-      <sharedItems containsBlank="1" longText="1"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Auteur" refreshedDate="44336.513236574072" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="49">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="Tâches"/>
@@ -745,7 +585,492 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Auteur" refreshedDate="44337.457857754627" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:I39" sheet="Tâches"/>
+  </cacheSource>
+  <cacheFields count="9">
+    <cacheField name="Index" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="38" count="38">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
+        <n v="8"/>
+        <n v="9"/>
+        <n v="10"/>
+        <n v="11"/>
+        <n v="12"/>
+        <n v="13"/>
+        <n v="14"/>
+        <n v="15"/>
+        <n v="16"/>
+        <n v="17"/>
+        <n v="18"/>
+        <n v="19"/>
+        <n v="20"/>
+        <n v="21"/>
+        <n v="22"/>
+        <n v="23"/>
+        <n v="24"/>
+        <n v="25"/>
+        <n v="26"/>
+        <n v="27"/>
+        <n v="28"/>
+        <n v="29"/>
+        <n v="30"/>
+        <n v="31"/>
+        <n v="32"/>
+        <n v="33"/>
+        <n v="34"/>
+        <n v="35"/>
+        <n v="36"/>
+        <n v="37"/>
+        <n v="38"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2021-05-03T00:00:00" maxDate="2021-05-18T00:00:00"/>
+    </cacheField>
+    <cacheField name="Début" numFmtId="20">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T08:03:00" maxDate="1899-12-30T16:04:00"/>
+    </cacheField>
+    <cacheField name="Fin" numFmtId="20">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T08:13:00" maxDate="1899-12-30T16:55:00"/>
+    </cacheField>
+    <cacheField name="Durée" numFmtId="20">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:03:00" maxDate="1899-12-30T03:22:00"/>
+    </cacheField>
+    <cacheField name="Type" numFmtId="0">
+      <sharedItems containsBlank="1" count="6">
+        <s v="Analyse"/>
+        <s v="Misc."/>
+        <s v="Documentation"/>
+        <s v="Conception"/>
+        <s v="Réalisation"/>
+        <m u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Tâche" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Commentaire" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sources" numFmtId="0">
+      <sharedItems containsBlank="1" longText="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="49">
+  <r>
+    <x v="0"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T08:08:00"/>
+    <d v="1899-12-30T08:13:00"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T08:14:00"/>
+    <d v="1899-12-30T08:25:00"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T08:30:00"/>
+    <d v="1899-12-30T08:58:00"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T09:00:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T09:55:00"/>
+    <d v="1899-12-30T10:18:00"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T10:19:00"/>
+    <d v="1899-12-30T10:41:00"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T10:42:00"/>
+    <d v="1899-12-30T10:45:00"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T10:46:00"/>
+    <d v="1899-12-30T11:17:00"/>
+    <x v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T11:18:00"/>
+    <d v="1899-12-30T11:31:00"/>
+    <x v="8"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T11:32:00"/>
+    <d v="1899-12-30T12:16:00"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:06:00"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T15:25:00"/>
+    <d v="1899-12-30T15:32:00"/>
+    <x v="11"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T15:33:00"/>
+    <d v="1899-12-30T16:03:00"/>
+    <x v="12"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <d v="2021-05-03T00:00:00"/>
+    <d v="1899-12-30T16:04:00"/>
+    <d v="1899-12-30T16:52:00"/>
+    <x v="13"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T08:05:00"/>
+    <d v="1899-12-30T08:32:00"/>
+    <x v="14"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T09:07:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <x v="15"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T14:08:00"/>
+    <x v="16"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T14:10:00"/>
+    <d v="1899-12-30T14:43:00"/>
+    <x v="17"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T14:44:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <x v="18"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <d v="2021-05-04T00:00:00"/>
+    <d v="1899-12-30T15:30:00"/>
+    <d v="1899-12-30T16:05:00"/>
+    <x v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T08:05:00"/>
+    <d v="1899-12-30T09:17:00"/>
+    <x v="19"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T09:17:00"/>
+    <d v="1899-12-30T09:36:00"/>
+    <x v="20"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T09:56:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <x v="21"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <d v="2021-05-06T00:00:00"/>
+    <d v="1899-12-30T13:32:00"/>
+    <d v="1899-12-30T16:50:00"/>
+    <x v="22"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <d v="2021-05-07T00:00:00"/>
+    <d v="1899-12-30T08:03:00"/>
+    <d v="1899-12-30T11:25:00"/>
+    <x v="23"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T08:18:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="24"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T09:51:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <x v="25"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:05:00"/>
+    <x v="26"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <d v="2021-05-10T00:00:00"/>
+    <d v="1899-12-30T15:20:00"/>
+    <d v="1899-12-30T16:55:00"/>
+    <x v="26"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T08:03:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="27"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T09:52:00"/>
+    <d v="1899-12-30T12:12:00"/>
+    <x v="28"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:06:00"/>
+    <x v="10"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <d v="2021-05-11T00:00:00"/>
+    <d v="1899-12-30T15:20:00"/>
+    <d v="1899-12-30T16:05:00"/>
+    <x v="29"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T08:15:00"/>
+    <d v="1899-12-30T08:52:00"/>
+    <x v="30"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="35"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T08:52:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="31"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T09:52:00"/>
+    <d v="1899-12-30T10:29:00"/>
+    <x v="30"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="37"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T10:30:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <x v="32"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="38"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T13:32:00"/>
+    <d v="1899-12-30T14:45:00"/>
+    <x v="33"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="39"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T14:45:00"/>
+    <d v="1899-12-30T15:15:00"/>
+    <x v="12"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="40"/>
+    <d v="2021-05-17T00:00:00"/>
+    <d v="1899-12-30T15:20:00"/>
+    <d v="1899-12-30T16:50:00"/>
+    <x v="34"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="41"/>
+    <d v="2021-05-18T00:00:00"/>
+    <d v="1899-12-30T08:02:00"/>
+    <d v="1899-12-30T08:42:00"/>
+    <x v="35"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="42"/>
+    <d v="2021-05-18T00:00:00"/>
+    <d v="1899-12-30T08:42:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="36"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="43"/>
+    <d v="2021-05-18T00:00:00"/>
+    <d v="1899-12-30T09:53:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <x v="37"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="44"/>
+    <d v="2021-05-20T00:00:00"/>
+    <d v="1899-12-30T08:01:00"/>
+    <d v="1899-12-30T08:15:00"/>
+    <x v="38"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="45"/>
+    <d v="2021-05-20T00:00:00"/>
+    <d v="1899-12-30T08:15:00"/>
+    <d v="1899-12-30T08:55:00"/>
+    <x v="35"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="46"/>
+    <d v="2021-05-20T00:00:00"/>
+    <d v="1899-12-30T09:00:00"/>
+    <d v="1899-12-30T09:36:00"/>
+    <x v="39"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="47"/>
+    <d v="2021-05-20T00:00:00"/>
+    <d v="1899-12-30T09:55:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <x v="28"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="48"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="40"/>
+    <x v="5"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="38">
   <r>
     <x v="0"/>
@@ -1168,405 +1493,8 @@
 </pivotCacheRecords>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="49">
-  <r>
-    <x v="0"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T08:08:00"/>
-    <d v="1899-12-30T08:13:00"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T08:14:00"/>
-    <d v="1899-12-30T08:25:00"/>
-    <x v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T08:30:00"/>
-    <d v="1899-12-30T08:58:00"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T09:00:00"/>
-    <d v="1899-12-30T09:35:00"/>
-    <x v="3"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T09:55:00"/>
-    <d v="1899-12-30T10:18:00"/>
-    <x v="4"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T10:19:00"/>
-    <d v="1899-12-30T10:41:00"/>
-    <x v="5"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T10:42:00"/>
-    <d v="1899-12-30T10:45:00"/>
-    <x v="6"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T10:46:00"/>
-    <d v="1899-12-30T11:17:00"/>
-    <x v="7"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T11:18:00"/>
-    <d v="1899-12-30T11:31:00"/>
-    <x v="8"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T11:32:00"/>
-    <d v="1899-12-30T12:16:00"/>
-    <x v="9"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T13:30:00"/>
-    <d v="1899-12-30T15:06:00"/>
-    <x v="10"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T15:25:00"/>
-    <d v="1899-12-30T15:32:00"/>
-    <x v="11"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="12"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T15:33:00"/>
-    <d v="1899-12-30T16:03:00"/>
-    <x v="12"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <d v="2021-05-03T00:00:00"/>
-    <d v="1899-12-30T16:04:00"/>
-    <d v="1899-12-30T16:52:00"/>
-    <x v="13"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <d v="2021-05-04T00:00:00"/>
-    <d v="1899-12-30T08:05:00"/>
-    <d v="1899-12-30T08:32:00"/>
-    <x v="14"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="15"/>
-    <d v="2021-05-04T00:00:00"/>
-    <d v="1899-12-30T09:07:00"/>
-    <d v="1899-12-30T09:35:00"/>
-    <x v="2"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="16"/>
-    <d v="2021-05-04T00:00:00"/>
-    <d v="1899-12-30T10:00:00"/>
-    <d v="1899-12-30T12:15:00"/>
-    <x v="15"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="17"/>
-    <d v="2021-05-04T00:00:00"/>
-    <d v="1899-12-30T13:30:00"/>
-    <d v="1899-12-30T14:08:00"/>
-    <x v="16"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="18"/>
-    <d v="2021-05-04T00:00:00"/>
-    <d v="1899-12-30T14:10:00"/>
-    <d v="1899-12-30T14:43:00"/>
-    <x v="17"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <d v="2021-05-04T00:00:00"/>
-    <d v="1899-12-30T14:44:00"/>
-    <d v="1899-12-30T15:00:00"/>
-    <x v="18"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="20"/>
-    <d v="2021-05-04T00:00:00"/>
-    <d v="1899-12-30T15:30:00"/>
-    <d v="1899-12-30T16:05:00"/>
-    <x v="3"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <d v="2021-05-06T00:00:00"/>
-    <d v="1899-12-30T08:05:00"/>
-    <d v="1899-12-30T09:17:00"/>
-    <x v="19"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="22"/>
-    <d v="2021-05-06T00:00:00"/>
-    <d v="1899-12-30T09:17:00"/>
-    <d v="1899-12-30T09:36:00"/>
-    <x v="20"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="23"/>
-    <d v="2021-05-06T00:00:00"/>
-    <d v="1899-12-30T09:56:00"/>
-    <d v="1899-12-30T12:15:00"/>
-    <x v="21"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="24"/>
-    <d v="2021-05-06T00:00:00"/>
-    <d v="1899-12-30T13:32:00"/>
-    <d v="1899-12-30T16:50:00"/>
-    <x v="22"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="25"/>
-    <d v="2021-05-07T00:00:00"/>
-    <d v="1899-12-30T08:03:00"/>
-    <d v="1899-12-30T11:25:00"/>
-    <x v="23"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="26"/>
-    <d v="2021-05-10T00:00:00"/>
-    <d v="1899-12-30T08:18:00"/>
-    <d v="1899-12-30T09:35:00"/>
-    <x v="24"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="27"/>
-    <d v="2021-05-10T00:00:00"/>
-    <d v="1899-12-30T09:51:00"/>
-    <d v="1899-12-30T12:15:00"/>
-    <x v="25"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="28"/>
-    <d v="2021-05-10T00:00:00"/>
-    <d v="1899-12-30T13:30:00"/>
-    <d v="1899-12-30T15:05:00"/>
-    <x v="26"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <d v="2021-05-10T00:00:00"/>
-    <d v="1899-12-30T15:20:00"/>
-    <d v="1899-12-30T16:55:00"/>
-    <x v="26"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="30"/>
-    <d v="2021-05-11T00:00:00"/>
-    <d v="1899-12-30T08:03:00"/>
-    <d v="1899-12-30T09:35:00"/>
-    <x v="27"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="31"/>
-    <d v="2021-05-11T00:00:00"/>
-    <d v="1899-12-30T09:52:00"/>
-    <d v="1899-12-30T12:12:00"/>
-    <x v="28"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="32"/>
-    <d v="2021-05-11T00:00:00"/>
-    <d v="1899-12-30T13:30:00"/>
-    <d v="1899-12-30T15:06:00"/>
-    <x v="10"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="33"/>
-    <d v="2021-05-11T00:00:00"/>
-    <d v="1899-12-30T15:20:00"/>
-    <d v="1899-12-30T16:05:00"/>
-    <x v="29"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="34"/>
-    <d v="2021-05-17T00:00:00"/>
-    <d v="1899-12-30T08:15:00"/>
-    <d v="1899-12-30T08:52:00"/>
-    <x v="30"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="35"/>
-    <d v="2021-05-17T00:00:00"/>
-    <d v="1899-12-30T08:52:00"/>
-    <d v="1899-12-30T09:35:00"/>
-    <x v="31"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="36"/>
-    <d v="2021-05-17T00:00:00"/>
-    <d v="1899-12-30T09:52:00"/>
-    <d v="1899-12-30T10:29:00"/>
-    <x v="30"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="37"/>
-    <d v="2021-05-17T00:00:00"/>
-    <d v="1899-12-30T10:30:00"/>
-    <d v="1899-12-30T12:15:00"/>
-    <x v="32"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="38"/>
-    <d v="2021-05-17T00:00:00"/>
-    <d v="1899-12-30T13:32:00"/>
-    <d v="1899-12-30T14:45:00"/>
-    <x v="33"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="39"/>
-    <d v="2021-05-17T00:00:00"/>
-    <d v="1899-12-30T14:45:00"/>
-    <d v="1899-12-30T15:15:00"/>
-    <x v="12"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="40"/>
-    <d v="2021-05-17T00:00:00"/>
-    <d v="1899-12-30T15:20:00"/>
-    <d v="1899-12-30T16:50:00"/>
-    <x v="34"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="41"/>
-    <d v="2021-05-18T00:00:00"/>
-    <d v="1899-12-30T08:02:00"/>
-    <d v="1899-12-30T08:42:00"/>
-    <x v="35"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="42"/>
-    <d v="2021-05-18T00:00:00"/>
-    <d v="1899-12-30T08:42:00"/>
-    <d v="1899-12-30T09:35:00"/>
-    <x v="36"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="43"/>
-    <d v="2021-05-18T00:00:00"/>
-    <d v="1899-12-30T09:53:00"/>
-    <d v="1899-12-30T12:15:00"/>
-    <x v="37"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="44"/>
-    <d v="2021-05-20T00:00:00"/>
-    <d v="1899-12-30T08:01:00"/>
-    <d v="1899-12-30T08:15:00"/>
-    <x v="38"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="45"/>
-    <d v="2021-05-20T00:00:00"/>
-    <d v="1899-12-30T08:15:00"/>
-    <d v="1899-12-30T08:55:00"/>
-    <x v="35"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="46"/>
-    <d v="2021-05-20T00:00:00"/>
-    <d v="1899-12-30T09:00:00"/>
-    <d v="1899-12-30T09:36:00"/>
-    <x v="39"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="47"/>
-    <d v="2021-05-20T00:00:00"/>
-    <d v="1899-12-30T09:55:00"/>
-    <d v="1899-12-30T12:15:00"/>
-    <x v="28"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="48"/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="40"/>
-    <x v="5"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -1723,7 +1651,7 @@
     <dataField name="Somme de Durée" fld="4" baseField="0" baseItem="7"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="33">
+    <format dxfId="6">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1737,7 +1665,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G53" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" countASubtotal="1">
@@ -2088,13 +2016,13 @@
     <dataField name="Somme de Durée" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="29">
+    <format dxfId="5">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="4">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="48">
@@ -2150,10 +2078,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="2">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="1">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2429,10 +2357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,7 +2429,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A49" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A62" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -2514,7 +2442,7 @@
         <v>0.35069444444444442</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E49" si="1">IF(OR(ISBLANK(D3),ISBLANK(C3)),"",D3-C3)</f>
+        <f t="shared" ref="E3:E52" si="1">IF(OR(ISBLANK(D3),ISBLANK(C3)),"",D3-C3)</f>
         <v>7.6388888888889173E-3</v>
       </c>
       <c r="F3" t="s">
@@ -3699,6 +3627,141 @@
       </c>
       <c r="G49" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>44337</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="1"/>
+        <v>6.5972222222222265E-2</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
+        <v>44337</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="1"/>
+        <v>4.9999999999999933E-2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B52" s="1">
+        <v>44337</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.4604166666666667</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.47638888888888892</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5972222222222221E-2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working simulation and In/Out canevas
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
     <pivotCache cacheId="5" r:id="rId6"/>
   </pivotCaches>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="79">
   <si>
     <t>Index</t>
   </si>
@@ -250,6 +250,27 @@
   </si>
   <si>
     <t>synérgie canevas et inputs</t>
+  </si>
+  <si>
+    <t>Fin de la synérgie entre canevas et inputs</t>
+  </si>
+  <si>
+    <t>Gestion de la caméra et épaisseur dynamique des câbles</t>
+  </si>
+  <si>
+    <t>Gestion des outputs du canevas</t>
+  </si>
+  <si>
+    <t>Simulation des portes logiques</t>
+  </si>
+  <si>
+    <t>Réparation des dégâts causés par Jonas</t>
+  </si>
+  <si>
+    <t>Correction de divers bugs liés aux câbles et à leur updates</t>
+  </si>
+  <si>
+    <t>Circuits récursifs non supportés. Custom components non supportés</t>
   </si>
 </sst>
 </file>
@@ -586,7 +607,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Auteur" refreshedDate="44337.457857754627" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Auteur" refreshedDate="44341.336910648148" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I39" sheet="Tâches"/>
   </cacheSource>
@@ -1665,7 +1686,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G53" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" countASubtotal="1">
@@ -2359,14 +2380,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="60" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="87.5703125" customWidth="1"/>
@@ -2442,7 +2464,7 @@
         <v>0.35069444444444442</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E52" si="1">IF(OR(ISBLANK(D3),ISBLANK(C3)),"",D3-C3)</f>
+        <f t="shared" ref="E3:E59" si="1">IF(OR(ISBLANK(D3),ISBLANK(C3)),"",D3-C3)</f>
         <v>7.6388888888889173E-3</v>
       </c>
       <c r="F3" t="s">
@@ -3604,7 +3626,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3629,7 +3651,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3654,7 +3676,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3679,7 +3701,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -3704,61 +3726,203 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="1">
+        <v>44341</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.33749999999999997</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.37361111111111112</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6111111111111149E-2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>44341</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.37361111111111112</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4583333333333337E-2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
+        <v>44341</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="1"/>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
+        <v>44341</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="1"/>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
+        <v>44341</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="1"/>
+        <v>4.7916666666666718E-2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" t="s">
+        <v>75</v>
+      </c>
+      <c r="H57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="1">
+        <v>44341</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.48680555555555555</v>
+      </c>
+      <c r="E58" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1805555555555514E-2</v>
+      </c>
+      <c r="F58" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
+        <v>44341</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.48680555555555555</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="E59" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0138888888888873E-2</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
+        <v>44341</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -3776,7 +3940,7 @@
           <x14:formula1>
             <xm:f>Sources!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F58</xm:sqref>
+          <xm:sqref>F2:F94</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Doxygen documentation & file saving & custom component simulation
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="93">
   <si>
     <t>Index</t>
   </si>
@@ -271,6 +271,48 @@
   </si>
   <si>
     <t>Circuits récursifs non supportés. Custom components non supportés</t>
+  </si>
+  <si>
+    <t>Dossier de réalisation</t>
+  </si>
+  <si>
+    <t>Management des composants dans le menu</t>
+  </si>
+  <si>
+    <t>Sauvegarde et composants</t>
+  </si>
+  <si>
+    <t>Tests divers</t>
+  </si>
+  <si>
+    <t>Sérialisation des components</t>
+  </si>
+  <si>
+    <t>Truth table computing</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/23905188/convert-an-integer-to-a-binary-string-with-leading-zeros</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/46408545/c-unity3d-json-parsing-failing-to-parse-json-into-c-sharp-object/46408705#46408705</t>
+  </si>
+  <si>
+    <t>Components instantiation</t>
+  </si>
+  <si>
+    <t>Custom components simulation</t>
+  </si>
+  <si>
+    <t>Works great afaik, need better testing thought</t>
+  </si>
+  <si>
+    <t>https://answers.unity.com/questions/717056/converting-binary-to-int.html</t>
+  </si>
+  <si>
+    <t>Small quality of life tweaks</t>
+  </si>
+  <si>
+    <t>Implementing Doxygen</t>
   </si>
 </sst>
 </file>
@@ -607,7 +649,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Auteur" refreshedDate="44341.336910648148" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Auteur" refreshedDate="44347.425115046295" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I39" sheet="Tâches"/>
   </cacheSource>
@@ -2378,10 +2420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,7 +2493,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A62" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A66" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -2464,7 +2506,7 @@
         <v>0.35069444444444442</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E59" si="1">IF(OR(ISBLANK(D3),ISBLANK(C3)),"",D3-C3)</f>
+        <f t="shared" ref="E3:E74" si="1">IF(OR(ISBLANK(D3),ISBLANK(C3)),"",D3-C3)</f>
         <v>7.6388888888889173E-3</v>
       </c>
       <c r="F3" t="s">
@@ -3915,17 +3957,398 @@
       <c r="C60" s="2">
         <v>0.5625</v>
       </c>
+      <c r="D60" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E60" s="2">
+        <f t="shared" si="1"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F60" t="s">
+        <v>11</v>
+      </c>
+      <c r="G60" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
+      <c r="B61" s="1">
+        <v>44341</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="E61" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1249999999999889E-2</v>
+      </c>
+      <c r="F61" t="s">
+        <v>11</v>
+      </c>
+      <c r="G61" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <v>44343</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E62" s="2">
+        <f t="shared" si="1"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F62" t="s">
+        <v>11</v>
+      </c>
+      <c r="G62" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
+        <v>44343</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="E63" s="2">
+        <f t="shared" si="1"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F63" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
+        <v>44344</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E64" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B65" s="1">
+        <v>44344</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="E65" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F65" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B66" s="1">
+        <v>44344</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E66" s="2">
+        <f t="shared" si="1"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="F66" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" ref="A67:A77" si="2">ROW()-1</f>
+        <v>66</v>
+      </c>
+      <c r="B67" s="1">
+        <v>44344</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="E67" s="2">
+        <f t="shared" si="1"/>
+        <v>6.5972222222222154E-2</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="B68" s="1">
+        <v>44347</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E68" s="2">
+        <f t="shared" si="1"/>
+        <v>6.3888888888888884E-2</v>
+      </c>
+      <c r="F68" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="B69" s="1">
+        <v>44347</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="E69" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8055555555555547E-2</v>
+      </c>
+      <c r="F69" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" t="s">
+        <v>83</v>
+      </c>
+      <c r="I69" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="1">
+        <v>44347</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.4916666666666667</v>
+      </c>
+      <c r="E70" s="2">
+        <f t="shared" si="1"/>
+        <v>6.3888888888888884E-2</v>
+      </c>
+      <c r="F70" t="s">
+        <v>11</v>
+      </c>
+      <c r="G70" t="s">
+        <v>84</v>
+      </c>
+      <c r="I70" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="1">
+        <v>44347</v>
+      </c>
+      <c r="C71" s="2">
+        <v>0.4916666666666667</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E71" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8749999999999933E-2</v>
+      </c>
+      <c r="F71" t="s">
+        <v>11</v>
+      </c>
+      <c r="G71" t="s">
+        <v>87</v>
+      </c>
+      <c r="I71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="1">
+        <v>44347</v>
+      </c>
+      <c r="C72" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0.61527777777777781</v>
+      </c>
+      <c r="E72" s="2">
+        <f t="shared" si="1"/>
+        <v>5.2777777777777812E-2</v>
+      </c>
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" t="s">
+        <v>88</v>
+      </c>
+      <c r="H72" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="1">
+        <v>44347</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.67083333333333339</v>
+      </c>
+      <c r="E73" s="2">
+        <f t="shared" si="1"/>
+        <v>5.4861111111111138E-2</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="1">
+        <v>44347</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0.67083333333333339</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.69027777777777777</v>
+      </c>
+      <c r="E74" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9444444444444375E-2</v>
+      </c>
+      <c r="F74" t="s">
+        <v>30</v>
+      </c>
+      <c r="G74" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="2"/>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes & up bar & comments
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -14,8 +14,8 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="10" r:id="rId5"/>
+    <pivotCache cacheId="14" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="101">
   <si>
     <t>Index</t>
   </si>
@@ -313,6 +313,30 @@
   </si>
   <si>
     <t>Implementing Doxygen</t>
+  </si>
+  <si>
+    <t>Delete et Edit des components dans le menu</t>
+  </si>
+  <si>
+    <t>Taille du rond de selection automatiquement ajustée à la camera</t>
+  </si>
+  <si>
+    <t>Travail sur la up bar</t>
+  </si>
+  <si>
+    <t>PNG export</t>
+  </si>
+  <si>
+    <t>https://docs.unity3d.com/ScriptReference/ScreenCapture.CaptureScreenshot.html?_gl=1*1r6m9c7*_ga*MTk4MDI3Nzg4MS4xNjEyMTgzMjg4*_ga_1S78EFL1W5*MTYyMjU0MTk3Ny44LjEuMTYyMjU0MzIwOS42MA..&amp;_ga=2.179108708.1172502326.1622448978-1980277881.1612183288</t>
+  </si>
+  <si>
+    <t>Pimp de l'appli</t>
+  </si>
+  <si>
+    <t>Autres options de la up bar</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
   </si>
 </sst>
 </file>
@@ -381,7 +405,25 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
@@ -417,13 +459,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Auteur" refreshedDate="44336.513236574072" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="49">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Auteur" refreshedDate="44348.580338194442" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="89">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="Tâches"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Index" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="48" count="49">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="88" count="89">
         <n v="1"/>
         <n v="2"/>
         <n v="3"/>
@@ -472,20 +514,60 @@
         <n v="46"/>
         <n v="47"/>
         <n v="48"/>
+        <n v="49"/>
+        <n v="50"/>
+        <n v="51"/>
+        <n v="52"/>
+        <n v="53"/>
+        <n v="54"/>
+        <n v="55"/>
+        <n v="56"/>
+        <n v="57"/>
+        <n v="58"/>
+        <n v="59"/>
+        <n v="60"/>
+        <n v="61"/>
+        <n v="62"/>
+        <n v="63"/>
+        <n v="64"/>
+        <n v="65"/>
+        <n v="66"/>
+        <n v="67"/>
+        <n v="68"/>
+        <n v="69"/>
+        <n v="70"/>
+        <n v="71"/>
+        <n v="72"/>
+        <n v="73"/>
+        <n v="74"/>
+        <n v="75"/>
+        <n v="76"/>
+        <n v="77"/>
+        <n v="78"/>
+        <n v="79"/>
+        <n v="80"/>
+        <n v="81"/>
+        <n v="82"/>
+        <n v="83"/>
+        <n v="84"/>
+        <n v="85"/>
+        <n v="86"/>
+        <n v="87"/>
+        <n v="88"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2021-05-03T00:00:00" maxDate="2021-05-21T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2021-05-03T00:00:00" maxDate="2021-06-02T00:00:00"/>
     </cacheField>
     <cacheField name="Début" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T08:01:00" maxDate="1899-12-30T16:04:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T08:00:00" maxDate="1899-12-30T16:06:00"/>
     </cacheField>
     <cacheField name="Fin" numFmtId="0">
       <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T08:13:00" maxDate="1899-12-30T16:55:00"/>
     </cacheField>
     <cacheField name="Durée" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T00:03:00" maxDate="1899-12-30T03:22:00" count="41">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T00:03:00" maxDate="1899-12-30T03:22:00" count="53">
         <d v="1899-12-30T00:05:00"/>
         <d v="1899-12-30T00:11:00"/>
         <d v="1899-12-30T00:28:00"/>
@@ -526,6 +608,18 @@
         <d v="1899-12-30T02:22:00"/>
         <d v="1899-12-30T00:14:00"/>
         <d v="1899-12-30T00:36:00"/>
+        <d v="1899-12-30T00:52:00"/>
+        <d v="1899-12-30T00:21:00"/>
+        <d v="1899-12-30T00:55:00"/>
+        <d v="1899-12-30T00:25:00"/>
+        <d v="1899-12-30T01:09:00"/>
+        <d v="1899-12-30T00:17:00"/>
+        <d v="1899-12-30T00:29:00"/>
+        <d v="1899-12-30T00:15:00"/>
+        <d v="1899-12-30T00:26:00"/>
+        <d v="1899-12-30T01:16:00"/>
+        <d v="1899-12-30T01:19:00"/>
+        <d v="1899-12-30T02:13:00"/>
         <m/>
       </sharedItems>
       <fieldGroup par="6" base="4">
@@ -597,12 +691,13 @@
       </fieldGroup>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
-      <sharedItems containsBlank="1" count="6">
+      <sharedItems containsBlank="1" count="7">
         <s v="Analyse"/>
         <s v="Misc."/>
         <s v="Documentation"/>
         <s v="Conception"/>
         <s v="Réalisation"/>
+        <s v="Tests"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -649,7 +744,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Auteur" refreshedDate="44347.425115046295" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Auteur" refreshedDate="44348.58051550926" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I39" sheet="Tâches"/>
   </cacheSource>
@@ -737,7 +832,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="49">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="89">
   <r>
     <x v="0"/>
     <d v="2021-05-03T00:00:00"/>
@@ -1124,11 +1219,331 @@
   </r>
   <r>
     <x v="48"/>
-    <m/>
-    <m/>
-    <m/>
+    <d v="2021-05-21T00:00:00"/>
+    <d v="1899-12-30T08:00:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="26"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="49"/>
+    <d v="2021-05-21T00:00:00"/>
+    <d v="1899-12-30T09:50:00"/>
+    <d v="1899-12-30T11:02:00"/>
+    <x v="19"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="50"/>
+    <d v="2021-05-21T00:00:00"/>
+    <d v="1899-12-30T11:03:00"/>
+    <d v="1899-12-30T11:26:00"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="51"/>
+    <d v="2021-05-25T00:00:00"/>
+    <d v="1899-12-30T08:06:00"/>
+    <d v="1899-12-30T08:58:00"/>
     <x v="40"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="52"/>
+    <d v="2021-05-25T00:00:00"/>
+    <d v="1899-12-30T08:58:00"/>
+    <d v="1899-12-30T09:19:00"/>
+    <x v="41"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="53"/>
+    <d v="2021-05-25T00:00:00"/>
+    <d v="1899-12-30T09:20:00"/>
+    <d v="1899-12-30T10:15:00"/>
+    <x v="42"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="54"/>
+    <d v="2021-05-25T00:00:00"/>
+    <d v="1899-12-30T09:50:00"/>
+    <d v="1899-12-30T10:15:00"/>
+    <x v="43"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="55"/>
+    <d v="2021-05-25T00:00:00"/>
+    <d v="1899-12-30T10:15:00"/>
+    <d v="1899-12-30T11:24:00"/>
+    <x v="44"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="56"/>
+    <d v="2021-05-25T00:00:00"/>
+    <d v="1899-12-30T11:24:00"/>
+    <d v="1899-12-30T11:41:00"/>
+    <x v="45"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="57"/>
+    <d v="2021-05-25T00:00:00"/>
+    <d v="1899-12-30T11:41:00"/>
+    <d v="1899-12-30T12:10:00"/>
+    <x v="46"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="58"/>
+    <d v="2021-05-25T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:05:00"/>
+    <x v="26"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="59"/>
+    <d v="2021-05-25T00:00:00"/>
+    <d v="1899-12-30T15:20:00"/>
+    <d v="1899-12-30T16:05:00"/>
+    <x v="29"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="60"/>
+    <d v="2021-05-27T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:05:00"/>
+    <x v="26"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="61"/>
+    <d v="2021-05-27T00:00:00"/>
+    <d v="1899-12-30T15:20:00"/>
+    <d v="1899-12-30T16:55:00"/>
+    <x v="26"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="62"/>
+    <d v="2021-05-28T00:00:00"/>
+    <d v="1899-12-30T08:05:00"/>
+    <d v="1899-12-30T08:20:00"/>
+    <x v="47"/>
     <x v="5"/>
+  </r>
+  <r>
+    <x v="63"/>
+    <d v="2021-05-28T00:00:00"/>
+    <d v="1899-12-30T08:20:00"/>
+    <d v="1899-12-30T08:50:00"/>
+    <x v="12"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="64"/>
+    <d v="2021-05-28T00:00:00"/>
+    <d v="1899-12-30T08:50:00"/>
+    <d v="1899-12-30T09:30:00"/>
+    <x v="35"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="65"/>
+    <d v="2021-05-28T00:00:00"/>
+    <d v="1899-12-30T09:50:00"/>
+    <d v="1899-12-30T11:25:00"/>
+    <x v="26"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="66"/>
+    <d v="2021-05-31T00:00:00"/>
+    <d v="1899-12-30T08:03:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="27"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="67"/>
+    <d v="2021-05-31T00:00:00"/>
+    <d v="1899-12-30T09:50:00"/>
+    <d v="1899-12-30T10:16:00"/>
+    <x v="48"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="68"/>
+    <d v="2021-05-31T00:00:00"/>
+    <d v="1899-12-30T10:16:00"/>
+    <d v="1899-12-30T11:48:00"/>
+    <x v="27"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="69"/>
+    <d v="2021-05-31T00:00:00"/>
+    <d v="1899-12-30T11:48:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <x v="14"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="70"/>
+    <d v="2021-05-31T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T14:46:00"/>
+    <x v="49"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="71"/>
+    <d v="2021-05-31T00:00:00"/>
+    <d v="1899-12-30T14:47:00"/>
+    <d v="1899-12-30T16:06:00"/>
+    <x v="50"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="72"/>
+    <d v="2021-05-31T00:00:00"/>
+    <d v="1899-12-30T16:06:00"/>
+    <d v="1899-12-30T16:34:00"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="73"/>
+    <d v="2021-06-01T00:00:00"/>
+    <d v="1899-12-30T08:05:00"/>
+    <d v="1899-12-30T09:24:00"/>
+    <x v="50"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="74"/>
+    <d v="2021-06-01T00:00:00"/>
+    <d v="1899-12-30T09:24:00"/>
+    <d v="1899-12-30T09:27:00"/>
+    <x v="6"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="75"/>
+    <d v="2021-06-01T00:00:00"/>
+    <d v="1899-12-30T09:28:00"/>
+    <d v="1899-12-30T09:35:00"/>
+    <x v="11"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="76"/>
+    <d v="2021-06-01T00:00:00"/>
+    <d v="1899-12-30T09:55:00"/>
+    <d v="1899-12-30T12:08:00"/>
+    <x v="51"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="77"/>
+    <d v="2021-06-01T00:00:00"/>
+    <d v="1899-12-30T12:08:00"/>
+    <d v="1899-12-30T12:15:00"/>
+    <x v="11"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="78"/>
+    <d v="2021-06-01T00:00:00"/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="79"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="80"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="81"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="82"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="83"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="84"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="85"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="86"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="87"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="88"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="52"/>
+    <x v="6"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -1557,7 +1972,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -1714,7 +2129,7 @@
     <dataField name="Somme de Durée" fld="4" baseField="0" baseItem="7"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="6">
+    <format dxfId="12">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1728,11 +2143,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:G53" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G82" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" countASubtotal="1">
-      <items count="50">
+      <items count="90">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -1781,7 +2196,47 @@
         <item x="45"/>
         <item x="46"/>
         <item x="47"/>
+        <item x="88"/>
         <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
         <item t="countA"/>
       </items>
     </pivotField>
@@ -1859,12 +2314,13 @@
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
-      <items count="7">
+      <items count="8">
         <item x="0"/>
         <item x="3"/>
         <item x="2"/>
         <item x="1"/>
         <item x="4"/>
+        <item h="1" x="6"/>
         <item h="1" x="5"/>
         <item t="default"/>
       </items>
@@ -1903,7 +2359,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="49">
+  <rowItems count="78">
     <i>
       <x/>
     </i>
@@ -2047,6 +2503,93 @@
     </i>
     <i>
       <x v="47"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="64"/>
+    </i>
+    <i>
+      <x v="65"/>
+    </i>
+    <i>
+      <x v="66"/>
+    </i>
+    <i>
+      <x v="67"/>
+    </i>
+    <i>
+      <x v="68"/>
+    </i>
+    <i>
+      <x v="69"/>
+    </i>
+    <i>
+      <x v="70"/>
+    </i>
+    <i>
+      <x v="71"/>
+    </i>
+    <i>
+      <x v="72"/>
+    </i>
+    <i>
+      <x v="73"/>
+    </i>
+    <i>
+      <x v="74"/>
+    </i>
+    <i>
+      <x v="75"/>
+    </i>
+    <i>
+      <x v="76"/>
+    </i>
+    <i>
+      <x v="77"/>
+    </i>
+    <i>
+      <x v="78"/>
     </i>
     <i t="grand">
       <x/>
@@ -2079,13 +2622,13 @@
     <dataField name="Somme de Durée" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="5">
+    <format dxfId="11">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="10">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="9">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="48">
@@ -2141,10 +2684,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="8">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="7">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2420,10 +2963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2506,7 +3049,7 @@
         <v>0.35069444444444442</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E74" si="1">IF(OR(ISBLANK(D3),ISBLANK(C3)),"",D3-C3)</f>
+        <f t="shared" ref="E3:E80" si="1">IF(OR(ISBLANK(D3),ISBLANK(C3)),"",D3-C3)</f>
         <v>7.6388888888889173E-3</v>
       </c>
       <c r="F3" t="s">
@@ -4123,7 +4666,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" ref="A67:A77" si="2">ROW()-1</f>
+        <f t="shared" ref="A67:A89" si="2">ROW()-1</f>
         <v>66</v>
       </c>
       <c r="B67" s="1">
@@ -4338,17 +4881,278 @@
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
+      <c r="B75" s="1">
+        <v>44348</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.39166666666666666</v>
+      </c>
+      <c r="E75" s="2">
+        <f t="shared" si="1"/>
+        <v>5.4861111111111083E-2</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
+      <c r="B76" s="1">
+        <v>44348</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0.39166666666666666</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0.39374999999999999</v>
+      </c>
+      <c r="E76" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333259E-3</v>
+      </c>
+      <c r="F76" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="2"/>
         <v>76</v>
+      </c>
+      <c r="B77" s="1">
+        <v>44348</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0.39444444444444443</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E77" s="2">
+        <f t="shared" si="1"/>
+        <v>4.8611111111111494E-3</v>
+      </c>
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="B78" s="1">
+        <v>44348</v>
+      </c>
+      <c r="C78" s="2">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="E78" s="2">
+        <f t="shared" si="1"/>
+        <v>9.2361111111111116E-2</v>
+      </c>
+      <c r="F78" t="s">
+        <v>11</v>
+      </c>
+      <c r="G78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="B79" s="1">
+        <v>44348</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="D79" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E79" s="2">
+        <f t="shared" si="1"/>
+        <v>4.8611111111110938E-3</v>
+      </c>
+      <c r="F79" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" t="s">
+        <v>96</v>
+      </c>
+      <c r="I79" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="B80" s="1">
+        <v>44348</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D80" s="2">
+        <v>0.59930555555555554</v>
+      </c>
+      <c r="E80" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6805555555555536E-2</v>
+      </c>
+      <c r="F80" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="B81" s="1">
+        <v>44348</v>
+      </c>
+      <c r="C81" s="2">
+        <v>0.59930555555555554</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="E81" s="2">
+        <f t="shared" ref="E81:E90" si="3">IF(OR(ISBLANK(D81),ISBLANK(C81)),"",D81-C81)</f>
+        <v>2.9861111111111116E-2</v>
+      </c>
+      <c r="F81" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="B82" s="1">
+        <v>44348</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="D82" s="2">
+        <v>0.66527777777777775</v>
+      </c>
+      <c r="E82" s="2">
+        <f t="shared" si="3"/>
+        <v>2.2916666666666696E-2</v>
+      </c>
+      <c r="F82" t="s">
+        <v>30</v>
+      </c>
+      <c r="G82" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="E83" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="E84" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="E85" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="E86" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="E87" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="E88" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="E89" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E90" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -4376,7 +5180,7 @@
   <dimension ref="A3:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4711,10 +5515,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G53"/>
+  <dimension ref="A3:G82"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4723,8 +5527,7 @@
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
     <col min="8" max="10" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
@@ -5483,26 +6286,461 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="4">
+        <v>49</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="G53" s="5">
+        <v>6.5972222222222224E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>50</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="G54" s="5">
+        <v>4.9999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>51</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="G55" s="5">
+        <v>1.5972222222222224E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>52</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="G56" s="5">
+        <v>3.6111111111111115E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>53</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5">
+        <v>1.4583333333333332E-2</v>
+      </c>
+      <c r="G57" s="5">
+        <v>1.4583333333333332E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>54</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="G58" s="5">
+        <v>3.8194444444444441E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>55</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="G59" s="5">
+        <v>1.7361111111111112E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>56</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5">
+        <v>4.7916666666666663E-2</v>
+      </c>
+      <c r="G60" s="5">
+        <v>4.7916666666666663E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>57</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="G61" s="5">
+        <v>1.1805555555555555E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>58</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="G62" s="5">
+        <v>2.013888888888889E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>59</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="G63" s="5">
+        <v>6.5972222222222224E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>60</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G64" s="5">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>61</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="G65" s="5">
+        <v>6.5972222222222224E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>62</v>
+      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="G66" s="5">
+        <v>6.5972222222222224E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>64</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>65</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G68" s="5">
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>66</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="G69" s="5">
+        <v>6.5972222222222224E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>67</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5">
+        <v>6.3888888888888884E-2</v>
+      </c>
+      <c r="G70" s="5">
+        <v>6.3888888888888884E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>68</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5">
+        <v>1.8055555555555557E-2</v>
+      </c>
+      <c r="G71" s="5">
+        <v>1.8055555555555557E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>69</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5">
+        <v>6.3888888888888884E-2</v>
+      </c>
+      <c r="G72" s="5">
+        <v>6.3888888888888884E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>70</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="G73" s="5">
+        <v>1.8749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>71</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="G74" s="5">
+        <v>5.2777777777777778E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>72</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="G75" s="5">
+        <v>5.486111111111111E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>73</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5">
+        <v>1.9444444444444445E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>74</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="G77" s="5">
+        <v>5.486111111111111E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>75</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="G78" s="5">
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>76</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="G79" s="5">
+        <v>4.8611111111111112E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>77</v>
+      </c>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5">
+        <v>9.2361111111111116E-2</v>
+      </c>
+      <c r="G80" s="5">
+        <v>9.2361111111111116E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>78</v>
+      </c>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="G81" s="5">
+        <v>4.8611111111111112E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B82" s="9">
         <v>8.1944444444444445E-2</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C82" s="9">
         <v>0.30277777777777781</v>
       </c>
-      <c r="D53" s="9">
-        <v>0.4826388888888889</v>
-      </c>
-      <c r="E53" s="9">
-        <v>0.11805555555555555</v>
-      </c>
-      <c r="F53" s="9">
-        <v>1.0993055555555555</v>
-      </c>
-      <c r="G53" s="9">
-        <v>2.0847222222222221</v>
+      <c r="D82" s="9">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="E82" s="9">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="F82" s="9">
+        <v>2.1715277777777779</v>
+      </c>
+      <c r="G82" s="9">
+        <v>3.1972222222222224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>